<commit_message>
added changes to files
</commit_message>
<xml_diff>
--- a/02-FormulasBasicas.xlsx
+++ b/02-FormulasBasicas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Excel\Clases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F999C8-E21A-4DCD-9574-FFC685D62A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C7ABEB-53BF-4CC6-A163-9144074B974D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10635" yWindow="2985" windowWidth="14700" windowHeight="12885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introducción" sheetId="1" r:id="rId1"/>
@@ -295,16 +295,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>209549</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>797615</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>74544</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>564949</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>134726</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>201268</xdr:rowOff>
+      <xdr:rowOff>314739</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -334,8 +334,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1841223" y="1399761"/>
-          <a:ext cx="2575139" cy="789333"/>
+          <a:off x="1559615" y="1325217"/>
+          <a:ext cx="3188524" cy="977348"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -927,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1091,12 +1091,12 @@
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="C18" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>2</v>
       </c>

</xml_diff>